<commit_message>
ładowanie do repozytorium głównego - cz.1
</commit_message>
<xml_diff>
--- a/sources/HD_projekt_kategorie kanałow.xlsx
+++ b/sources/HD_projekt_kategorie kanałow.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ITI\Audience Measurement\Pliki źródłowe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radek\source\repos\HD\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D90676A4-7706-4EC5-9A72-A53EB4BED93B}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0DFFE5-55C3-4575-8755-28180A2F7CBB}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1425" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="grupy mediowe" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -1736,9 +1736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B142"/>
   <sheetViews>
-    <sheetView topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="B145" sqref="B145"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2889,8 +2887,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
-      <selection activeCell="F199" sqref="F199"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>